<commit_message>
add associacao ao grupo aC
</commit_message>
<xml_diff>
--- a/sgtpy/database/saftgamma_database.xlsx
+++ b/sgtpy/database/saftgamma_database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dfs\APPS\CDI\rm-sgtpy\sgtpy\sgtpy\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E96F6B1-694F-4735-A30B-14CED77E25BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F4E217-750D-4172-80F9-8AA8593D1E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="groups" sheetId="1" r:id="rId1"/>
@@ -419,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -440,6 +440,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -824,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60:M60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3451,22 +3452,22 @@
       <c r="G60" s="6">
         <v>6</v>
       </c>
-      <c r="H60">
-        <v>0</v>
-      </c>
-      <c r="I60">
-        <v>0</v>
-      </c>
-      <c r="J60">
-        <v>0</v>
-      </c>
-      <c r="K60">
-        <v>0</v>
-      </c>
-      <c r="L60">
-        <v>0</v>
-      </c>
-      <c r="M60">
+      <c r="H60" s="16">
+        <v>1</v>
+      </c>
+      <c r="I60" s="16">
+        <v>0</v>
+      </c>
+      <c r="J60" s="16">
+        <v>1</v>
+      </c>
+      <c r="K60" s="16">
+        <v>0</v>
+      </c>
+      <c r="L60" s="16">
+        <v>0</v>
+      </c>
+      <c r="M60" s="16">
         <v>0</v>
       </c>
       <c r="N60">
@@ -3486,7 +3487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F346"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>

</xml_diff>